<commit_message>
Updated selected files in scrapers/src and scrapers/datas
</commit_message>
<xml_diff>
--- a/scrapers/data/links/Companies.xlsx
+++ b/scrapers/data/links/Companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/supriyajadhav/Documents/Capstone/scrapers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/supriyajadhav/Documents/Capstone/AgentMADS/scrapers/data/links/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30CEA51E-4FC2-4B42-9988-7BE9720D73CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712DCFB5-48BC-9143-9EF0-7465170B1E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{84F7A25D-3132-DD42-AF5D-F54C3FC6EB91}"/>
+    <workbookView xWindow="1900" yWindow="6640" windowWidth="27640" windowHeight="15300" xr2:uid="{84F7A25D-3132-DD42-AF5D-F54C3FC6EB91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Company Name</t>
   </si>
@@ -72,6 +72,102 @@
   </si>
   <si>
     <t>shreecem</t>
+  </si>
+  <si>
+    <t>Tata Motors</t>
+  </si>
+  <si>
+    <t>PC Jeweller</t>
+  </si>
+  <si>
+    <t>Vakrangee</t>
+  </si>
+  <si>
+    <t>Jubilant Foodworks</t>
+  </si>
+  <si>
+    <t>Vakrangee Limited-$</t>
+  </si>
+  <si>
+    <t>vakrangee</t>
+  </si>
+  <si>
+    <t>vakrangee-limited</t>
+  </si>
+  <si>
+    <t>tata-motors-ltd</t>
+  </si>
+  <si>
+    <t>tatamotors</t>
+  </si>
+  <si>
+    <t>TATA MOTORS LTD.</t>
+  </si>
+  <si>
+    <t>pc-jeweller-ltd</t>
+  </si>
+  <si>
+    <t>pcjeweller</t>
+  </si>
+  <si>
+    <t>PC JEWELLER LTD.</t>
+  </si>
+  <si>
+    <t>Jubilant FoodWorks Ltd</t>
+  </si>
+  <si>
+    <t>jubilant-foodworks-ltd</t>
+  </si>
+  <si>
+    <t>jublfood</t>
+  </si>
+  <si>
+    <t>Paytm</t>
+  </si>
+  <si>
+    <t>One 97 Communications Ltd</t>
+  </si>
+  <si>
+    <t>one-97-communications-ltd</t>
+  </si>
+  <si>
+    <t>paytm</t>
+  </si>
+  <si>
+    <t>Sanghvi Movers</t>
+  </si>
+  <si>
+    <t>sanghvimov</t>
+  </si>
+  <si>
+    <t>sanghvi-movers-ltd</t>
+  </si>
+  <si>
+    <t>SANGHVI MOVERS LTD.</t>
+  </si>
+  <si>
+    <t>MGL</t>
+  </si>
+  <si>
+    <t>Religare</t>
+  </si>
+  <si>
+    <t>Mahanagar Gas Ltd</t>
+  </si>
+  <si>
+    <t>mgl</t>
+  </si>
+  <si>
+    <t>mahanagar-gas-ltd</t>
+  </si>
+  <si>
+    <t>RELIGARE ENTERPRISES LTD.</t>
+  </si>
+  <si>
+    <t>religare</t>
+  </si>
+  <si>
+    <t>religare-enterprises-ltd</t>
   </si>
 </sst>
 </file>
@@ -81,8 +177,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -92,9 +196,8 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,15 +220,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,71 +547,282 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47519520-3084-1544-A90A-A6B93BF8EB1D}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
+        <v>500387</v>
+      </c>
+      <c r="C2" s="1">
         <v>324875</v>
       </c>
-      <c r="C2" s="2">
-        <v>500387</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2">
         <v>45627</v>
       </c>
-      <c r="F2" s="2">
+      <c r="H2" s="1">
         <v>124</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>500570</v>
+      </c>
+      <c r="C3">
+        <v>327610</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2">
+        <v>45627</v>
+      </c>
+      <c r="H3" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>534809</v>
+      </c>
+      <c r="C4">
+        <v>327230</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2">
+        <v>45627</v>
+      </c>
+      <c r="H4" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>511431</v>
+      </c>
+      <c r="C5">
+        <v>325794</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="2">
+        <v>45627</v>
+      </c>
+      <c r="H5" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>533155</v>
+      </c>
+      <c r="C6">
+        <v>326075</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="2">
+        <v>45627</v>
+      </c>
+      <c r="H6" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>543396</v>
+      </c>
+      <c r="C7">
+        <v>325689</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2">
+        <v>45627</v>
+      </c>
+      <c r="H7" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>530073</v>
+      </c>
+      <c r="C8">
+        <v>327162</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="2">
+        <v>45627</v>
+      </c>
+      <c r="H8" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>539957</v>
+      </c>
+      <c r="C9">
+        <v>326504</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="2">
+        <v>45627</v>
+      </c>
+      <c r="H9" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>532915</v>
+      </c>
+      <c r="C10">
+        <v>328115</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="2">
+        <v>45627</v>
+      </c>
+      <c r="H10" s="1">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>